<commit_message>
Issue 3 update add gantt chart
</commit_message>
<xml_diff>
--- a/doc/新要件定義/ガント チャート.xlsx
+++ b/doc/新要件定義/ガント チャート.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F001EEBD-BD1F-4B7E-B505-A25B85659470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2C6919-88E4-4A78-A2A4-9FB7374E9EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2036,7 +2036,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="91" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2868,7 +2868,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="38">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>29</v>

</xml_diff>